<commit_message>
Minor accuracy improvement to io-model/DCSoCbIC
</commit_message>
<xml_diff>
--- a/InputData/io-model/DCSoCbIC/Domestic Content Share of Consumption by ISIC Code.xlsx
+++ b/InputData/io-model/DCSoCbIC/Domestic Content Share of Consumption by ISIC Code.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\io-model\DPSbIC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\io-model\DCSoCbIC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BCA139-5DE3-4C18-82FD-7E66F8C3D5B5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D4DA87-6E86-4EDF-B9E4-570BE5704F2E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4035" yWindow="375" windowWidth="24765" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -885,6 +885,55 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
@@ -915,67 +964,18 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="6" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="4" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="4" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="8" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1378,17 +1378,17 @@
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="51" t="s">
+      <c r="A28" s="37" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="37" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="37" t="s">
         <v>175</v>
       </c>
     </row>
@@ -1423,8 +1423,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC40CF3-8B3B-41DC-A935-B8F6C9564C97}">
   <dimension ref="A1:AU50"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView showGridLines="0" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="AR13" sqref="AR13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1460,222 +1460,222 @@
       </c>
     </row>
     <row r="3" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="24" t="s">
+      <c r="B3" s="39"/>
+      <c r="C3" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="25"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="25"/>
-      <c r="L3" s="25"/>
-      <c r="M3" s="25"/>
-      <c r="N3" s="25"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="25"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="25"/>
-      <c r="V3" s="25"/>
-      <c r="W3" s="25"/>
-      <c r="X3" s="25"/>
-      <c r="Y3" s="25"/>
-      <c r="Z3" s="25"/>
-      <c r="AA3" s="25"/>
-      <c r="AB3" s="25"/>
-      <c r="AC3" s="25"/>
-      <c r="AD3" s="25"/>
-      <c r="AE3" s="25"/>
-      <c r="AF3" s="25"/>
-      <c r="AG3" s="25"/>
-      <c r="AH3" s="25"/>
-      <c r="AI3" s="25"/>
-      <c r="AJ3" s="25"/>
-      <c r="AK3" s="25"/>
-      <c r="AL3" s="25"/>
-      <c r="AM3" s="25"/>
-      <c r="AN3" s="25"/>
-      <c r="AO3" s="25"/>
-      <c r="AP3" s="25"/>
-      <c r="AQ3" s="25"/>
-      <c r="AR3" s="25"/>
-      <c r="AS3" s="25"/>
-      <c r="AT3" s="25"/>
-      <c r="AU3" s="26"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
+      <c r="N3" s="46"/>
+      <c r="O3" s="46"/>
+      <c r="P3" s="46"/>
+      <c r="Q3" s="46"/>
+      <c r="R3" s="46"/>
+      <c r="S3" s="46"/>
+      <c r="T3" s="46"/>
+      <c r="U3" s="46"/>
+      <c r="V3" s="46"/>
+      <c r="W3" s="46"/>
+      <c r="X3" s="46"/>
+      <c r="Y3" s="46"/>
+      <c r="Z3" s="46"/>
+      <c r="AA3" s="46"/>
+      <c r="AB3" s="46"/>
+      <c r="AC3" s="46"/>
+      <c r="AD3" s="46"/>
+      <c r="AE3" s="46"/>
+      <c r="AF3" s="46"/>
+      <c r="AG3" s="46"/>
+      <c r="AH3" s="46"/>
+      <c r="AI3" s="46"/>
+      <c r="AJ3" s="46"/>
+      <c r="AK3" s="46"/>
+      <c r="AL3" s="46"/>
+      <c r="AM3" s="46"/>
+      <c r="AN3" s="46"/>
+      <c r="AO3" s="46"/>
+      <c r="AP3" s="46"/>
+      <c r="AQ3" s="46"/>
+      <c r="AR3" s="46"/>
+      <c r="AS3" s="46"/>
+      <c r="AT3" s="46"/>
+      <c r="AU3" s="47"/>
     </row>
     <row r="4" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="19" t="s">
+      <c r="B4" s="39"/>
+      <c r="C4" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
-      <c r="S4" s="20"/>
-      <c r="T4" s="20"/>
-      <c r="U4" s="20"/>
-      <c r="V4" s="20"/>
-      <c r="W4" s="20"/>
-      <c r="X4" s="20"/>
-      <c r="Y4" s="20"/>
-      <c r="Z4" s="20"/>
-      <c r="AA4" s="20"/>
-      <c r="AB4" s="20"/>
-      <c r="AC4" s="20"/>
-      <c r="AD4" s="20"/>
-      <c r="AE4" s="20"/>
-      <c r="AF4" s="20"/>
-      <c r="AG4" s="20"/>
-      <c r="AH4" s="20"/>
-      <c r="AI4" s="20"/>
-      <c r="AJ4" s="20"/>
-      <c r="AK4" s="20"/>
-      <c r="AL4" s="20"/>
-      <c r="AM4" s="20"/>
-      <c r="AN4" s="20"/>
-      <c r="AO4" s="20"/>
-      <c r="AP4" s="20"/>
-      <c r="AQ4" s="20"/>
-      <c r="AR4" s="20"/>
-      <c r="AS4" s="20"/>
-      <c r="AT4" s="20"/>
-      <c r="AU4" s="21"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="41"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="41"/>
+      <c r="Q4" s="41"/>
+      <c r="R4" s="41"/>
+      <c r="S4" s="41"/>
+      <c r="T4" s="41"/>
+      <c r="U4" s="41"/>
+      <c r="V4" s="41"/>
+      <c r="W4" s="41"/>
+      <c r="X4" s="41"/>
+      <c r="Y4" s="41"/>
+      <c r="Z4" s="41"/>
+      <c r="AA4" s="41"/>
+      <c r="AB4" s="41"/>
+      <c r="AC4" s="41"/>
+      <c r="AD4" s="41"/>
+      <c r="AE4" s="41"/>
+      <c r="AF4" s="41"/>
+      <c r="AG4" s="41"/>
+      <c r="AH4" s="41"/>
+      <c r="AI4" s="41"/>
+      <c r="AJ4" s="41"/>
+      <c r="AK4" s="41"/>
+      <c r="AL4" s="41"/>
+      <c r="AM4" s="41"/>
+      <c r="AN4" s="41"/>
+      <c r="AO4" s="41"/>
+      <c r="AP4" s="41"/>
+      <c r="AQ4" s="41"/>
+      <c r="AR4" s="41"/>
+      <c r="AS4" s="41"/>
+      <c r="AT4" s="41"/>
+      <c r="AU4" s="42"/>
     </row>
     <row r="5" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="19" t="s">
+      <c r="B5" s="39"/>
+      <c r="C5" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="20"/>
-      <c r="T5" s="20"/>
-      <c r="U5" s="20"/>
-      <c r="V5" s="20"/>
-      <c r="W5" s="20"/>
-      <c r="X5" s="20"/>
-      <c r="Y5" s="20"/>
-      <c r="Z5" s="20"/>
-      <c r="AA5" s="20"/>
-      <c r="AB5" s="20"/>
-      <c r="AC5" s="20"/>
-      <c r="AD5" s="20"/>
-      <c r="AE5" s="20"/>
-      <c r="AF5" s="20"/>
-      <c r="AG5" s="20"/>
-      <c r="AH5" s="20"/>
-      <c r="AI5" s="20"/>
-      <c r="AJ5" s="20"/>
-      <c r="AK5" s="20"/>
-      <c r="AL5" s="20"/>
-      <c r="AM5" s="20"/>
-      <c r="AN5" s="20"/>
-      <c r="AO5" s="20"/>
-      <c r="AP5" s="20"/>
-      <c r="AQ5" s="20"/>
-      <c r="AR5" s="20"/>
-      <c r="AS5" s="20"/>
-      <c r="AT5" s="20"/>
-      <c r="AU5" s="21"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
+      <c r="Q5" s="41"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="41"/>
+      <c r="T5" s="41"/>
+      <c r="U5" s="41"/>
+      <c r="V5" s="41"/>
+      <c r="W5" s="41"/>
+      <c r="X5" s="41"/>
+      <c r="Y5" s="41"/>
+      <c r="Z5" s="41"/>
+      <c r="AA5" s="41"/>
+      <c r="AB5" s="41"/>
+      <c r="AC5" s="41"/>
+      <c r="AD5" s="41"/>
+      <c r="AE5" s="41"/>
+      <c r="AF5" s="41"/>
+      <c r="AG5" s="41"/>
+      <c r="AH5" s="41"/>
+      <c r="AI5" s="41"/>
+      <c r="AJ5" s="41"/>
+      <c r="AK5" s="41"/>
+      <c r="AL5" s="41"/>
+      <c r="AM5" s="41"/>
+      <c r="AN5" s="41"/>
+      <c r="AO5" s="41"/>
+      <c r="AP5" s="41"/>
+      <c r="AQ5" s="41"/>
+      <c r="AR5" s="41"/>
+      <c r="AS5" s="41"/>
+      <c r="AT5" s="41"/>
+      <c r="AU5" s="42"/>
     </row>
     <row r="6" spans="1:47" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="38" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="19" t="s">
+      <c r="B6" s="39"/>
+      <c r="C6" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="20"/>
-      <c r="S6" s="20"/>
-      <c r="T6" s="20"/>
-      <c r="U6" s="20"/>
-      <c r="V6" s="20"/>
-      <c r="W6" s="20"/>
-      <c r="X6" s="20"/>
-      <c r="Y6" s="20"/>
-      <c r="Z6" s="20"/>
-      <c r="AA6" s="20"/>
-      <c r="AB6" s="20"/>
-      <c r="AC6" s="20"/>
-      <c r="AD6" s="20"/>
-      <c r="AE6" s="20"/>
-      <c r="AF6" s="20"/>
-      <c r="AG6" s="20"/>
-      <c r="AH6" s="20"/>
-      <c r="AI6" s="20"/>
-      <c r="AJ6" s="20"/>
-      <c r="AK6" s="20"/>
-      <c r="AL6" s="20"/>
-      <c r="AM6" s="20"/>
-      <c r="AN6" s="20"/>
-      <c r="AO6" s="20"/>
-      <c r="AP6" s="20"/>
-      <c r="AQ6" s="20"/>
-      <c r="AR6" s="20"/>
-      <c r="AS6" s="20"/>
-      <c r="AT6" s="20"/>
-      <c r="AU6" s="21"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
+      <c r="G6" s="41"/>
+      <c r="H6" s="41"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="41"/>
+      <c r="P6" s="41"/>
+      <c r="Q6" s="41"/>
+      <c r="R6" s="41"/>
+      <c r="S6" s="41"/>
+      <c r="T6" s="41"/>
+      <c r="U6" s="41"/>
+      <c r="V6" s="41"/>
+      <c r="W6" s="41"/>
+      <c r="X6" s="41"/>
+      <c r="Y6" s="41"/>
+      <c r="Z6" s="41"/>
+      <c r="AA6" s="41"/>
+      <c r="AB6" s="41"/>
+      <c r="AC6" s="41"/>
+      <c r="AD6" s="41"/>
+      <c r="AE6" s="41"/>
+      <c r="AF6" s="41"/>
+      <c r="AG6" s="41"/>
+      <c r="AH6" s="41"/>
+      <c r="AI6" s="41"/>
+      <c r="AJ6" s="41"/>
+      <c r="AK6" s="41"/>
+      <c r="AL6" s="41"/>
+      <c r="AM6" s="41"/>
+      <c r="AN6" s="41"/>
+      <c r="AO6" s="41"/>
+      <c r="AP6" s="41"/>
+      <c r="AQ6" s="41"/>
+      <c r="AR6" s="41"/>
+      <c r="AS6" s="41"/>
+      <c r="AT6" s="41"/>
+      <c r="AU6" s="42"/>
     </row>
     <row r="7" spans="1:47" ht="126" x14ac:dyDescent="0.2">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="43" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="23"/>
+      <c r="B7" s="44"/>
       <c r="C7" s="8" t="s">
         <v>52</v>
       </c>
@@ -7855,484 +7855,484 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" style="27" customWidth="1"/>
-    <col min="2" max="2" width="2.42578125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="27"/>
+    <col min="1" max="1" width="27.42578125" style="17" customWidth="1"/>
+    <col min="2" max="2" width="2.42578125" style="17" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="17" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="40" t="e">
+      <c r="A1" s="26" t="e">
         <f ca="1">DotStatQuery(B1)</f>
         <v>#NAME?</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="26" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="25" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="52.5" x14ac:dyDescent="0.2">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="42" t="s">
+      <c r="B3" s="49"/>
+      <c r="C3" s="28" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="37"/>
-      <c r="C4" s="41" t="s">
+      <c r="B4" s="49"/>
+      <c r="C4" s="27" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="38" t="s">
+      <c r="A5" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="41" t="s">
+      <c r="B5" s="49"/>
+      <c r="C5" s="27" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="41" t="s">
+      <c r="B6" s="49"/>
+      <c r="C6" s="27" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="52.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="B7" s="35"/>
-      <c r="C7" s="34" t="s">
+      <c r="B7" s="51"/>
+      <c r="C7" s="24" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="33" t="s">
+      <c r="A8" s="23" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="30" t="s">
+      <c r="B8" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="20" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="B9" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="29">
+      <c r="B9" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="19">
         <v>9.14</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="B10" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" s="32">
+      <c r="B10" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="22">
         <v>2.96</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="31" t="s">
+      <c r="A11" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="B11" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C11" s="29">
+      <c r="B11" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="19">
         <v>4.17</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="31" t="s">
+      <c r="A12" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="B12" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C12" s="32">
+      <c r="B12" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="22">
         <v>4.87</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A13" s="31" t="s">
+      <c r="A13" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="B13" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="29">
+      <c r="B13" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="19">
         <v>10.56</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="B14" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="32">
+      <c r="B14" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="22">
         <v>16.34</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="31" t="s">
+      <c r="A15" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="B15" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="29">
+      <c r="B15" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="19">
         <v>14.2</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="31" t="s">
+      <c r="A16" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="B16" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16" s="32">
+      <c r="B16" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="22">
         <v>13.16</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="31" t="s">
+      <c r="A17" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="29">
+      <c r="B17" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="19">
         <v>26.63</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A18" s="31" t="s">
+      <c r="A18" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="B18" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="32">
+      <c r="B18" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="22">
         <v>10.58</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A19" s="31" t="s">
+      <c r="A19" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="B19" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="29">
+      <c r="B19" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="19">
         <v>14.98</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A20" s="31" t="s">
+      <c r="A20" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="B20" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" s="32">
+      <c r="B20" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="22">
         <v>10.47</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="B21" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21" s="29">
+      <c r="B21" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="19">
         <v>17.71</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="31" t="s">
+      <c r="A22" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="B22" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="32">
+      <c r="B22" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="22">
         <v>16.260000000000002</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A23" s="31" t="s">
+      <c r="A23" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="B23" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23" s="29">
+      <c r="B23" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="19">
         <v>8.2200000000000006</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="31" t="s">
+      <c r="A24" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="B24" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C24" s="32">
+      <c r="B24" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="22">
         <v>17.48</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A25" s="31" t="s">
+      <c r="A25" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="B25" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C25" s="29">
+      <c r="B25" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25" s="19">
         <v>19.36</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A26" s="31" t="s">
+      <c r="A26" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="B26" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C26" s="32">
+      <c r="B26" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="22">
         <v>25.14</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A27" s="31" t="s">
+      <c r="A27" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="B27" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C27" s="29">
+      <c r="B27" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" s="19">
         <v>16</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="42" x14ac:dyDescent="0.25">
-      <c r="A28" s="31" t="s">
+      <c r="A28" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="B28" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="32">
+      <c r="B28" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28" s="22">
         <v>12.84</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="31" t="s">
+      <c r="A29" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="B29" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C29" s="29">
+      <c r="B29" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C29" s="19">
         <v>7.68</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="B30" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C30" s="32">
+      <c r="B30" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30" s="22">
         <v>10.93</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="B31" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="29">
+      <c r="B31" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31" s="19">
         <v>3.49</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="21" x14ac:dyDescent="0.25">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="B32" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32" s="32">
+      <c r="B32" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="22">
         <v>7.9</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A33" s="31" t="s">
+      <c r="A33" s="21" t="s">
         <v>122</v>
       </c>
-      <c r="B33" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C33" s="29">
+      <c r="B33" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="19">
         <v>5.82</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A34" s="31" t="s">
+      <c r="A34" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="B34" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34" s="32">
+      <c r="B34" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="22">
         <v>2.68</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A35" s="31" t="s">
+      <c r="A35" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="B35" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C35" s="29">
+      <c r="B35" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35" s="19">
         <v>7.81</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A36" s="31" t="s">
+      <c r="A36" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="B36" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C36" s="32">
+      <c r="B36" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36" s="22">
         <v>4.9400000000000004</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A37" s="31" t="s">
+      <c r="A37" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="B37" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37" s="29">
+      <c r="B37" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37" s="19">
         <v>2.8</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="31" t="s">
+      <c r="A38" s="21" t="s">
         <v>127</v>
       </c>
-      <c r="B38" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38" s="32">
+      <c r="B38" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38" s="22">
         <v>1.59</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A39" s="31" t="s">
+      <c r="A39" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="B39" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" s="29">
+      <c r="B39" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C39" s="19">
         <v>3.82</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="48" t="s">
+      <c r="A40" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="B40" s="49" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40" s="50">
+      <c r="B40" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C40" s="36">
         <f>C39</f>
         <v>3.82</v>
       </c>
-      <c r="D40" s="47" t="s">
+      <c r="D40" s="33" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="31" t="s">
+      <c r="A41" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="B41" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="32">
+      <c r="B41" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C41" s="22">
         <v>2.3199999999999998</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="21" x14ac:dyDescent="0.25">
-      <c r="A42" s="31" t="s">
+      <c r="A42" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="B42" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C42" s="29">
+      <c r="B42" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C42" s="19">
         <v>4.7699999999999996</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A43" s="31" t="s">
+      <c r="A43" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="B43" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C43" s="32">
+      <c r="B43" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C43" s="22">
         <v>4.79</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="13.5" x14ac:dyDescent="0.25">
-      <c r="A44" s="31" t="s">
+      <c r="A44" s="21" t="s">
         <v>142</v>
       </c>
-      <c r="B44" s="30" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44" s="29">
+      <c r="B44" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" s="19">
         <v>9.92</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A45" s="28" t="s">
+      <c r="A45" s="18" t="s">
         <v>160</v>
       </c>
     </row>
@@ -8358,7 +8358,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97A28A8A-BF96-4EEF-AD22-FD46200C7D59}">
   <dimension ref="A1:AK9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8480,147 +8482,147 @@
       <c r="A2" t="s">
         <v>144</v>
       </c>
-      <c r="B2" s="44">
+      <c r="B2" s="30">
         <f>'OECD TTL'!C49</f>
         <v>455757.4</v>
       </c>
-      <c r="C2" s="44">
+      <c r="C2" s="30">
         <f>'OECD TTL'!D49</f>
         <v>293671.09999999998</v>
       </c>
-      <c r="D2" s="44">
+      <c r="D2" s="30">
         <f>'OECD TTL'!E49</f>
         <v>64889.3</v>
       </c>
-      <c r="E2" s="44">
+      <c r="E2" s="30">
         <f>'OECD TTL'!F49</f>
         <v>87786.1</v>
       </c>
-      <c r="F2" s="44">
+      <c r="F2" s="30">
         <f>'OECD TTL'!G49</f>
         <v>935808.4</v>
       </c>
-      <c r="G2" s="44">
+      <c r="G2" s="30">
         <f>'OECD TTL'!H49</f>
         <v>87018.8</v>
       </c>
-      <c r="H2" s="44">
+      <c r="H2" s="30">
         <f>'OECD TTL'!I49</f>
         <v>98613</v>
       </c>
-      <c r="I2" s="44">
+      <c r="I2" s="30">
         <f>'OECD TTL'!J49</f>
         <v>269203.3</v>
       </c>
-      <c r="J2" s="44">
+      <c r="J2" s="30">
         <f>'OECD TTL'!K49</f>
         <v>490118.1</v>
       </c>
-      <c r="K2" s="44">
+      <c r="K2" s="30">
         <f>'OECD TTL'!L49</f>
         <v>785327</v>
       </c>
-      <c r="L2" s="44">
+      <c r="L2" s="30">
         <f>'OECD TTL'!M49</f>
         <v>230983</v>
       </c>
-      <c r="M2" s="44">
+      <c r="M2" s="30">
         <f>'OECD TTL'!N49</f>
         <v>119491.4</v>
       </c>
-      <c r="N2" s="44">
+      <c r="N2" s="30">
         <f>'OECD TTL'!O49</f>
         <v>225243.7</v>
       </c>
-      <c r="O2" s="44">
+      <c r="O2" s="30">
         <f>'OECD TTL'!P49</f>
         <v>367581.1</v>
       </c>
-      <c r="P2" s="44">
+      <c r="P2" s="30">
         <f>'OECD TTL'!Q49</f>
         <v>380874.8</v>
       </c>
-      <c r="Q2" s="44">
+      <c r="Q2" s="30">
         <f>'OECD TTL'!R49</f>
         <v>125254.1</v>
       </c>
-      <c r="R2" s="44">
+      <c r="R2" s="30">
         <f>'OECD TTL'!S49</f>
         <v>380878.6</v>
       </c>
-      <c r="S2" s="44">
+      <c r="S2" s="30">
         <f>'OECD TTL'!T49</f>
         <v>666400</v>
       </c>
-      <c r="T2" s="44">
+      <c r="T2" s="30">
         <f>'OECD TTL'!U49</f>
         <v>334983</v>
       </c>
-      <c r="U2" s="44">
+      <c r="U2" s="30">
         <f>'OECD TTL'!V49</f>
         <v>246719.5</v>
       </c>
-      <c r="V2" s="44">
+      <c r="V2" s="30">
         <f>'OECD TTL'!W49</f>
         <v>475620.1</v>
       </c>
-      <c r="W2" s="44">
+      <c r="W2" s="30">
         <f>'OECD TTL'!X49</f>
         <v>1351706.6</v>
       </c>
-      <c r="X2" s="44">
+      <c r="X2" s="30">
         <f>'OECD TTL'!Y49</f>
         <v>2970593.4</v>
       </c>
-      <c r="Y2" s="44">
+      <c r="Y2" s="30">
         <f>'OECD TTL'!Z49</f>
         <v>1121923.2</v>
       </c>
-      <c r="Z2" s="44">
+      <c r="Z2" s="30">
         <f>'OECD TTL'!AA49</f>
         <v>917753.9</v>
       </c>
-      <c r="AA2" s="44">
+      <c r="AA2" s="30">
         <f>'OECD TTL'!AB49</f>
         <v>657592</v>
       </c>
-      <c r="AB2" s="44">
+      <c r="AB2" s="30">
         <f>'OECD TTL'!AC49</f>
         <v>635977.4</v>
       </c>
-      <c r="AC2" s="44">
+      <c r="AC2" s="30">
         <f>'OECD TTL'!AD49</f>
         <v>578097.80000000005</v>
       </c>
-      <c r="AD2" s="44">
+      <c r="AD2" s="30">
         <f>'OECD TTL'!AE49</f>
         <v>2294683.9</v>
       </c>
-      <c r="AE2" s="44">
+      <c r="AE2" s="30">
         <f>'OECD TTL'!AF49</f>
         <v>3002385.4</v>
       </c>
-      <c r="AF2" s="44">
+      <c r="AF2" s="30">
         <f>'OECD TTL'!AG49</f>
         <v>3345452.3</v>
       </c>
-      <c r="AG2" s="44">
+      <c r="AG2" s="30">
         <f>'OECD TTL'!AH49</f>
         <v>2508797.2999999998</v>
       </c>
-      <c r="AH2" s="44">
+      <c r="AH2" s="30">
         <f>'OECD TTL'!AI49</f>
         <v>1304057.3999999999</v>
       </c>
-      <c r="AI2" s="44">
+      <c r="AI2" s="30">
         <f>'OECD TTL'!AJ49</f>
         <v>2187438.6</v>
       </c>
-      <c r="AJ2" s="44">
+      <c r="AJ2" s="30">
         <f>'OECD TTL'!AK49</f>
         <v>800816.1</v>
       </c>
-      <c r="AK2" s="44">
+      <c r="AK2" s="30">
         <f>'OECD TTL'!AL49</f>
         <v>21351.7</v>
       </c>
@@ -8629,113 +8631,113 @@
       <c r="A3" t="s">
         <v>143</v>
       </c>
-      <c r="B3" s="44">
-        <f t="array" ref="B3:AK3">-TRANSPOSE('OECD TTL'!AU9:AU44)</f>
-        <v>37816</v>
-      </c>
-      <c r="C3" s="44">
-        <v>161022.9</v>
-      </c>
-      <c r="D3" s="44">
-        <v>7908.2</v>
-      </c>
-      <c r="E3" s="44">
-        <v>1554.4</v>
-      </c>
-      <c r="F3" s="44">
-        <v>84486.2</v>
-      </c>
-      <c r="G3" s="44">
-        <v>145065.5</v>
-      </c>
-      <c r="H3" s="44">
-        <v>16997.3</v>
-      </c>
-      <c r="I3" s="44">
-        <v>23813.7</v>
-      </c>
-      <c r="J3" s="44">
-        <v>55734.3</v>
-      </c>
-      <c r="K3" s="44">
-        <v>165140.70000000001</v>
-      </c>
-      <c r="L3" s="44">
-        <v>49527.3</v>
-      </c>
-      <c r="M3" s="44">
-        <v>26110.400000000001</v>
-      </c>
-      <c r="N3" s="44">
-        <v>77529.899999999994</v>
-      </c>
-      <c r="O3" s="44">
-        <v>65502.400000000001</v>
-      </c>
-      <c r="P3" s="44">
-        <v>240846.5</v>
-      </c>
-      <c r="Q3" s="44">
-        <v>88431.1</v>
-      </c>
-      <c r="R3" s="44">
-        <v>128475.8</v>
-      </c>
-      <c r="S3" s="44">
-        <v>306727.09999999998</v>
-      </c>
-      <c r="T3" s="44">
-        <v>61444.6</v>
-      </c>
-      <c r="U3" s="44">
-        <v>99643.3</v>
-      </c>
-      <c r="V3" s="44">
-        <v>4933</v>
-      </c>
-      <c r="W3" s="44">
-        <v>1563</v>
-      </c>
-      <c r="X3" s="44">
-        <v>197714.9</v>
-      </c>
-      <c r="Y3" s="44">
-        <v>127601.9</v>
-      </c>
-      <c r="Z3" s="44">
-        <v>51797.3</v>
-      </c>
-      <c r="AA3" s="44">
-        <v>11993.5</v>
-      </c>
-      <c r="AB3" s="44">
-        <v>3766.8</v>
-      </c>
-      <c r="AC3" s="44">
-        <v>62979.199999999997</v>
-      </c>
-      <c r="AD3" s="44">
-        <v>56936.7</v>
-      </c>
-      <c r="AE3" s="44">
-        <v>10003</v>
-      </c>
-      <c r="AF3" s="44">
-        <v>132575.6</v>
-      </c>
-      <c r="AG3" s="44">
-        <v>2410.8000000000002</v>
-      </c>
-      <c r="AH3" s="44">
-        <v>11121.3</v>
-      </c>
-      <c r="AI3" s="44">
-        <v>2867.1</v>
-      </c>
-      <c r="AJ3" s="44">
-        <v>8872.6</v>
-      </c>
-      <c r="AK3" s="44">
+      <c r="B3" s="30">
+        <f t="array" ref="B3:AK3">-TRANSPOSE('OECD TTL'!AU9:AU44)+TRANSPOSE('OECD TTL'!AR9:AR44)</f>
+        <v>38981.599999999999</v>
+      </c>
+      <c r="C3" s="30">
+        <v>161086.1</v>
+      </c>
+      <c r="D3" s="30">
+        <v>7924.7</v>
+      </c>
+      <c r="E3" s="30">
+        <v>1559</v>
+      </c>
+      <c r="F3" s="30">
+        <v>88860.4</v>
+      </c>
+      <c r="G3" s="30">
+        <v>147429.4</v>
+      </c>
+      <c r="H3" s="30">
+        <v>17160.5</v>
+      </c>
+      <c r="I3" s="30">
+        <v>24284.799999999999</v>
+      </c>
+      <c r="J3" s="30">
+        <v>56773.3</v>
+      </c>
+      <c r="K3" s="30">
+        <v>166123.1</v>
+      </c>
+      <c r="L3" s="30">
+        <v>49582.8</v>
+      </c>
+      <c r="M3" s="30">
+        <v>26138.800000000003</v>
+      </c>
+      <c r="N3" s="30">
+        <v>77592</v>
+      </c>
+      <c r="O3" s="30">
+        <v>65569.899999999994</v>
+      </c>
+      <c r="P3" s="30">
+        <v>241417.3</v>
+      </c>
+      <c r="Q3" s="30">
+        <v>88653.8</v>
+      </c>
+      <c r="R3" s="30">
+        <v>128575.5</v>
+      </c>
+      <c r="S3" s="30">
+        <v>307102.3</v>
+      </c>
+      <c r="T3" s="30">
+        <v>61471.199999999997</v>
+      </c>
+      <c r="U3" s="30">
+        <v>101432</v>
+      </c>
+      <c r="V3" s="30">
+        <v>5034.2</v>
+      </c>
+      <c r="W3" s="30">
+        <v>1728</v>
+      </c>
+      <c r="X3" s="30">
+        <v>202854.9</v>
+      </c>
+      <c r="Y3" s="30">
+        <v>142205.9</v>
+      </c>
+      <c r="Z3" s="30">
+        <v>103059.3</v>
+      </c>
+      <c r="AA3" s="30">
+        <v>12786.4</v>
+      </c>
+      <c r="AB3" s="30">
+        <v>6386.3</v>
+      </c>
+      <c r="AC3" s="30">
+        <v>63090.399999999994</v>
+      </c>
+      <c r="AD3" s="30">
+        <v>59237.299999999996</v>
+      </c>
+      <c r="AE3" s="30">
+        <v>17008.3</v>
+      </c>
+      <c r="AF3" s="30">
+        <v>135958.30000000002</v>
+      </c>
+      <c r="AG3" s="30">
+        <v>2765.2000000000003</v>
+      </c>
+      <c r="AH3" s="30">
+        <v>17957.099999999999</v>
+      </c>
+      <c r="AI3" s="30">
+        <v>4957.7999999999993</v>
+      </c>
+      <c r="AJ3" s="30">
+        <v>16046.6</v>
+      </c>
+      <c r="AK3" s="30">
         <v>0</v>
       </c>
     </row>
@@ -8743,113 +8745,113 @@
       <c r="A4" t="s">
         <v>148</v>
       </c>
-      <c r="B4" s="44">
-        <f t="array" ref="B4:AK4">TRANSPOSE('OECD TTL'!AT9:AT44)</f>
-        <v>49518.6</v>
-      </c>
-      <c r="C4" s="44">
-        <v>18940.2</v>
-      </c>
-      <c r="D4" s="44">
-        <v>6342.5</v>
-      </c>
-      <c r="E4" s="44">
-        <v>2983.2</v>
-      </c>
-      <c r="F4" s="44">
-        <v>60181.5</v>
-      </c>
-      <c r="G4" s="44">
-        <v>8336.7999999999993</v>
-      </c>
-      <c r="H4" s="44">
-        <v>6289.2</v>
-      </c>
-      <c r="I4" s="44">
-        <v>30004.1</v>
-      </c>
-      <c r="J4" s="44">
-        <v>83383.3</v>
-      </c>
-      <c r="K4" s="44">
-        <v>136712.4</v>
-      </c>
-      <c r="L4" s="44">
-        <v>27545.8</v>
-      </c>
-      <c r="M4" s="44">
-        <v>10452.299999999999</v>
-      </c>
-      <c r="N4" s="44">
-        <v>43658.1</v>
-      </c>
-      <c r="O4" s="44">
-        <v>43973.8</v>
-      </c>
-      <c r="P4" s="44">
-        <v>75532.2</v>
-      </c>
-      <c r="Q4" s="44">
-        <v>26067.1</v>
-      </c>
-      <c r="R4" s="44">
-        <v>96005.1</v>
-      </c>
-      <c r="S4" s="44">
-        <v>105195.7</v>
-      </c>
-      <c r="T4" s="44">
-        <v>129693.6</v>
-      </c>
-      <c r="U4" s="44">
-        <v>21561.4</v>
-      </c>
-      <c r="V4" s="44">
-        <v>319.2</v>
-      </c>
-      <c r="W4" s="44">
+      <c r="B4" s="30">
+        <f t="array" ref="B4:AK4">TRANSPOSE('OECD TTL'!AT9:AT44)+TRANSPOSE('OECD TTL'!AS9:AS44)</f>
+        <v>51438.7</v>
+      </c>
+      <c r="C4" s="30">
+        <v>19010</v>
+      </c>
+      <c r="D4" s="30">
+        <v>6346.3</v>
+      </c>
+      <c r="E4" s="30">
+        <v>2984.1</v>
+      </c>
+      <c r="F4" s="30">
+        <v>67551.8</v>
+      </c>
+      <c r="G4" s="30">
+        <v>9569.6999999999989</v>
+      </c>
+      <c r="H4" s="30">
+        <v>6494.2</v>
+      </c>
+      <c r="I4" s="30">
+        <v>31165.899999999998</v>
+      </c>
+      <c r="J4" s="30">
+        <v>86119.5</v>
+      </c>
+      <c r="K4" s="30">
+        <v>138630.79999999999</v>
+      </c>
+      <c r="L4" s="30">
+        <v>27607.200000000001</v>
+      </c>
+      <c r="M4" s="30">
+        <v>10470</v>
+      </c>
+      <c r="N4" s="30">
+        <v>43660.9</v>
+      </c>
+      <c r="O4" s="30">
+        <v>44057.4</v>
+      </c>
+      <c r="P4" s="30">
+        <v>76723.3</v>
+      </c>
+      <c r="Q4" s="30">
+        <v>26399.399999999998</v>
+      </c>
+      <c r="R4" s="30">
+        <v>96063</v>
+      </c>
+      <c r="S4" s="30">
+        <v>105852.3</v>
+      </c>
+      <c r="T4" s="30">
+        <v>129731.20000000001</v>
+      </c>
+      <c r="U4" s="30">
+        <v>24010.400000000001</v>
+      </c>
+      <c r="V4" s="30">
+        <v>338.3</v>
+      </c>
+      <c r="W4" s="30">
         <v>10.9</v>
       </c>
-      <c r="X4" s="44">
-        <v>247263.3</v>
-      </c>
-      <c r="Y4" s="44">
-        <v>114350</v>
-      </c>
-      <c r="Z4" s="44">
-        <v>359.8</v>
-      </c>
-      <c r="AA4" s="44">
-        <v>51784.5</v>
-      </c>
-      <c r="AB4" s="44">
-        <v>19652.7</v>
-      </c>
-      <c r="AC4" s="44">
-        <v>29688.2</v>
-      </c>
-      <c r="AD4" s="44">
-        <v>137386.4</v>
-      </c>
-      <c r="AE4" s="44">
-        <v>4065.6</v>
-      </c>
-      <c r="AF4" s="44">
-        <v>250423.6</v>
-      </c>
-      <c r="AG4" s="44">
-        <v>0</v>
-      </c>
-      <c r="AH4" s="44">
-        <v>1550.8</v>
-      </c>
-      <c r="AI4" s="44">
-        <v>3.9</v>
-      </c>
-      <c r="AJ4" s="44">
-        <v>2915.5</v>
-      </c>
-      <c r="AK4" s="44">
+      <c r="X4" s="30">
+        <v>257715.5</v>
+      </c>
+      <c r="Y4" s="30">
+        <v>140375.9</v>
+      </c>
+      <c r="Z4" s="30">
+        <v>57852.5</v>
+      </c>
+      <c r="AA4" s="30">
+        <v>52684.1</v>
+      </c>
+      <c r="AB4" s="30">
+        <v>24353.599999999999</v>
+      </c>
+      <c r="AC4" s="30">
+        <v>29945.8</v>
+      </c>
+      <c r="AD4" s="30">
+        <v>141539.29999999999</v>
+      </c>
+      <c r="AE4" s="30">
+        <v>13957.9</v>
+      </c>
+      <c r="AF4" s="30">
+        <v>256262</v>
+      </c>
+      <c r="AG4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="30">
+        <v>26614.899999999998</v>
+      </c>
+      <c r="AI4" s="30">
+        <v>3081.9</v>
+      </c>
+      <c r="AJ4" s="30">
+        <v>15264.2</v>
+      </c>
+      <c r="AK4" s="30">
         <v>0</v>
       </c>
     </row>
@@ -8857,147 +8859,147 @@
       <c r="A5" t="s">
         <v>147</v>
       </c>
-      <c r="B5" s="44">
+      <c r="B5" s="30">
         <f>B2+B3-B4</f>
-        <v>444054.80000000005</v>
-      </c>
-      <c r="C5" s="44">
+        <v>443300.3</v>
+      </c>
+      <c r="C5" s="30">
         <f t="shared" ref="C5:AK5" si="0">C2+C3-C4</f>
-        <v>435753.8</v>
-      </c>
-      <c r="D5" s="44">
+        <v>435747.19999999995</v>
+      </c>
+      <c r="D5" s="30">
         <f t="shared" si="0"/>
-        <v>66455</v>
-      </c>
-      <c r="E5" s="44">
+        <v>66467.7</v>
+      </c>
+      <c r="E5" s="30">
         <f t="shared" si="0"/>
-        <v>86357.3</v>
-      </c>
-      <c r="F5" s="44">
+        <v>86361</v>
+      </c>
+      <c r="F5" s="30">
         <f t="shared" si="0"/>
-        <v>960113.1</v>
-      </c>
-      <c r="G5" s="44">
+        <v>957117</v>
+      </c>
+      <c r="G5" s="30">
         <f t="shared" si="0"/>
-        <v>223747.5</v>
-      </c>
-      <c r="H5" s="44">
+        <v>224878.5</v>
+      </c>
+      <c r="H5" s="30">
         <f t="shared" si="0"/>
-        <v>109321.1</v>
-      </c>
-      <c r="I5" s="44">
+        <v>109279.3</v>
+      </c>
+      <c r="I5" s="30">
         <f t="shared" si="0"/>
-        <v>263012.90000000002</v>
-      </c>
-      <c r="J5" s="44">
+        <v>262322.19999999995</v>
+      </c>
+      <c r="J5" s="30">
         <f t="shared" si="0"/>
-        <v>462469.10000000003</v>
-      </c>
-      <c r="K5" s="44">
+        <v>460771.9</v>
+      </c>
+      <c r="K5" s="30">
         <f t="shared" si="0"/>
-        <v>813755.29999999993</v>
-      </c>
-      <c r="L5" s="44">
+        <v>812819.3</v>
+      </c>
+      <c r="L5" s="30">
         <f t="shared" si="0"/>
-        <v>252964.5</v>
-      </c>
-      <c r="M5" s="44">
+        <v>252958.59999999998</v>
+      </c>
+      <c r="M5" s="30">
         <f t="shared" si="0"/>
-        <v>135149.5</v>
-      </c>
-      <c r="N5" s="44">
+        <v>135160.20000000001</v>
+      </c>
+      <c r="N5" s="30">
         <f t="shared" si="0"/>
-        <v>259115.49999999997</v>
-      </c>
-      <c r="O5" s="44">
+        <v>259174.80000000002</v>
+      </c>
+      <c r="O5" s="30">
         <f t="shared" si="0"/>
-        <v>389109.7</v>
-      </c>
-      <c r="P5" s="44">
+        <v>389093.6</v>
+      </c>
+      <c r="P5" s="30">
         <f t="shared" si="0"/>
-        <v>546189.10000000009</v>
-      </c>
-      <c r="Q5" s="44">
+        <v>545568.79999999993</v>
+      </c>
+      <c r="Q5" s="30">
         <f t="shared" si="0"/>
-        <v>187618.1</v>
-      </c>
-      <c r="R5" s="44">
+        <v>187508.50000000003</v>
+      </c>
+      <c r="R5" s="30">
         <f t="shared" si="0"/>
-        <v>413349.29999999993</v>
-      </c>
-      <c r="S5" s="44">
+        <v>413391.1</v>
+      </c>
+      <c r="S5" s="30">
         <f t="shared" si="0"/>
-        <v>867931.4</v>
-      </c>
-      <c r="T5" s="44">
+        <v>867650</v>
+      </c>
+      <c r="T5" s="30">
         <f t="shared" si="0"/>
-        <v>266734</v>
-      </c>
-      <c r="U5" s="44">
+        <v>266723</v>
+      </c>
+      <c r="U5" s="30">
         <f t="shared" si="0"/>
-        <v>324801.39999999997</v>
-      </c>
-      <c r="V5" s="44">
+        <v>324141.09999999998</v>
+      </c>
+      <c r="V5" s="30">
         <f t="shared" si="0"/>
-        <v>480233.89999999997</v>
-      </c>
-      <c r="W5" s="44">
+        <v>480316</v>
+      </c>
+      <c r="W5" s="30">
         <f t="shared" si="0"/>
-        <v>1353258.7000000002</v>
-      </c>
-      <c r="X5" s="44">
+        <v>1353423.7000000002</v>
+      </c>
+      <c r="X5" s="30">
         <f t="shared" si="0"/>
-        <v>2921045</v>
-      </c>
-      <c r="Y5" s="44">
+        <v>2915732.8</v>
+      </c>
+      <c r="Y5" s="30">
         <f t="shared" si="0"/>
-        <v>1135175.0999999999</v>
-      </c>
-      <c r="Z5" s="44">
+        <v>1123753.2</v>
+      </c>
+      <c r="Z5" s="30">
         <f t="shared" si="0"/>
-        <v>969191.4</v>
-      </c>
-      <c r="AA5" s="44">
+        <v>962960.70000000007</v>
+      </c>
+      <c r="AA5" s="30">
         <f t="shared" si="0"/>
-        <v>617801</v>
-      </c>
-      <c r="AB5" s="44">
+        <v>617694.30000000005</v>
+      </c>
+      <c r="AB5" s="30">
         <f t="shared" si="0"/>
-        <v>620091.50000000012</v>
-      </c>
-      <c r="AC5" s="44">
+        <v>618010.10000000009</v>
+      </c>
+      <c r="AC5" s="30">
         <f t="shared" si="0"/>
-        <v>611388.80000000005</v>
-      </c>
-      <c r="AD5" s="44">
+        <v>611242.4</v>
+      </c>
+      <c r="AD5" s="30">
         <f t="shared" si="0"/>
-        <v>2214234.2000000002</v>
-      </c>
-      <c r="AE5" s="44">
+        <v>2212381.9</v>
+      </c>
+      <c r="AE5" s="30">
         <f t="shared" si="0"/>
-        <v>3008322.8</v>
-      </c>
-      <c r="AF5" s="44">
+        <v>3005435.8</v>
+      </c>
+      <c r="AF5" s="30">
         <f t="shared" si="0"/>
-        <v>3227604.3</v>
-      </c>
-      <c r="AG5" s="44">
+        <v>3225148.5999999996</v>
+      </c>
+      <c r="AG5" s="30">
         <f t="shared" si="0"/>
-        <v>2511208.0999999996</v>
-      </c>
-      <c r="AH5" s="44">
+        <v>2511562.5</v>
+      </c>
+      <c r="AH5" s="30">
         <f t="shared" si="0"/>
-        <v>1313627.8999999999</v>
-      </c>
-      <c r="AI5" s="44">
+        <v>1295399.6000000001</v>
+      </c>
+      <c r="AI5" s="30">
         <f t="shared" si="0"/>
-        <v>2190301.8000000003</v>
-      </c>
-      <c r="AJ5" s="44">
+        <v>2189314.5</v>
+      </c>
+      <c r="AJ5" s="30">
         <f t="shared" si="0"/>
-        <v>806773.2</v>
-      </c>
-      <c r="AK5" s="44">
+        <v>801598.5</v>
+      </c>
+      <c r="AK5" s="30">
         <f t="shared" si="0"/>
         <v>21351.7</v>
       </c>
@@ -9006,113 +9008,113 @@
       <c r="A6" t="s">
         <v>154</v>
       </c>
-      <c r="B6" s="45">
+      <c r="B6" s="31">
         <f t="array" ref="B6:AJ6">TRANSPOSE('OECD ICESHR'!C9:C43)/100</f>
         <v>9.1400000000000009E-2</v>
       </c>
-      <c r="C6" s="45">
+      <c r="C6" s="31">
         <v>2.9600000000000001E-2</v>
       </c>
-      <c r="D6" s="45">
+      <c r="D6" s="31">
         <v>4.1700000000000001E-2</v>
       </c>
-      <c r="E6" s="45">
+      <c r="E6" s="31">
         <v>4.87E-2</v>
       </c>
-      <c r="F6" s="45">
+      <c r="F6" s="31">
         <v>0.1056</v>
       </c>
-      <c r="G6" s="45">
+      <c r="G6" s="31">
         <v>0.16339999999999999</v>
       </c>
-      <c r="H6" s="45">
+      <c r="H6" s="31">
         <v>0.14199999999999999</v>
       </c>
-      <c r="I6" s="45">
+      <c r="I6" s="31">
         <v>0.13159999999999999</v>
       </c>
-      <c r="J6" s="45">
+      <c r="J6" s="31">
         <v>0.26629999999999998</v>
       </c>
-      <c r="K6" s="45">
+      <c r="K6" s="31">
         <v>0.10580000000000001</v>
       </c>
-      <c r="L6" s="45">
+      <c r="L6" s="31">
         <v>0.14980000000000002</v>
       </c>
-      <c r="M6" s="45">
+      <c r="M6" s="31">
         <v>0.1047</v>
       </c>
-      <c r="N6" s="45">
+      <c r="N6" s="31">
         <v>0.17710000000000001</v>
       </c>
-      <c r="O6" s="45">
+      <c r="O6" s="31">
         <v>0.16260000000000002</v>
       </c>
-      <c r="P6" s="45">
+      <c r="P6" s="31">
         <v>8.2200000000000009E-2</v>
       </c>
-      <c r="Q6" s="45">
+      <c r="Q6" s="31">
         <v>0.17480000000000001</v>
       </c>
-      <c r="R6" s="45">
+      <c r="R6" s="31">
         <v>0.19359999999999999</v>
       </c>
-      <c r="S6" s="45">
+      <c r="S6" s="31">
         <v>0.25140000000000001</v>
       </c>
-      <c r="T6" s="45">
+      <c r="T6" s="31">
         <v>0.16</v>
       </c>
-      <c r="U6" s="45">
+      <c r="U6" s="31">
         <v>0.12839999999999999</v>
       </c>
-      <c r="V6" s="45">
+      <c r="V6" s="31">
         <v>7.6799999999999993E-2</v>
       </c>
-      <c r="W6" s="45">
+      <c r="W6" s="31">
         <v>0.10929999999999999</v>
       </c>
-      <c r="X6" s="45">
+      <c r="X6" s="31">
         <v>3.49E-2</v>
       </c>
-      <c r="Y6" s="45">
+      <c r="Y6" s="31">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="Z6" s="45">
+      <c r="Z6" s="31">
         <v>5.8200000000000002E-2</v>
       </c>
-      <c r="AA6" s="45">
+      <c r="AA6" s="31">
         <v>2.6800000000000001E-2</v>
       </c>
-      <c r="AB6" s="45">
+      <c r="AB6" s="31">
         <v>7.8100000000000003E-2</v>
       </c>
-      <c r="AC6" s="45">
+      <c r="AC6" s="31">
         <v>4.9400000000000006E-2</v>
       </c>
-      <c r="AD6" s="45">
+      <c r="AD6" s="31">
         <v>2.7999999999999997E-2</v>
       </c>
-      <c r="AE6" s="45">
+      <c r="AE6" s="31">
         <v>1.5900000000000001E-2</v>
       </c>
-      <c r="AF6" s="45">
+      <c r="AF6" s="31">
         <v>3.8199999999999998E-2</v>
       </c>
-      <c r="AG6" s="45">
+      <c r="AG6" s="31">
         <v>3.8199999999999998E-2</v>
       </c>
-      <c r="AH6" s="45">
+      <c r="AH6" s="31">
         <v>2.3199999999999998E-2</v>
       </c>
-      <c r="AI6" s="45">
+      <c r="AI6" s="31">
         <v>4.7699999999999992E-2</v>
       </c>
-      <c r="AJ6" s="45">
+      <c r="AJ6" s="31">
         <v>4.7899999999999998E-2</v>
       </c>
-      <c r="AK6" s="45">
+      <c r="AK6" s="31">
         <v>0</v>
       </c>
     </row>
@@ -9120,147 +9122,147 @@
       <c r="A7" t="s">
         <v>155</v>
       </c>
-      <c r="B7" s="44">
+      <c r="B7" s="30">
         <f>B3*(1-B6)</f>
-        <v>34359.617599999998</v>
-      </c>
-      <c r="C7" s="44">
+        <v>35418.681759999999</v>
+      </c>
+      <c r="C7" s="30">
         <f t="shared" ref="C7:AK7" si="1">C3*(1-C6)</f>
-        <v>156256.62216</v>
-      </c>
-      <c r="D7" s="44">
+        <v>156317.95144</v>
+      </c>
+      <c r="D7" s="30">
         <f t="shared" si="1"/>
-        <v>7578.4280600000002</v>
-      </c>
-      <c r="E7" s="44">
+        <v>7594.2400100000004</v>
+      </c>
+      <c r="E7" s="30">
         <f t="shared" si="1"/>
-        <v>1478.70072</v>
-      </c>
-      <c r="F7" s="44">
+        <v>1483.0767000000001</v>
+      </c>
+      <c r="F7" s="30">
         <f t="shared" si="1"/>
-        <v>75564.457280000002</v>
-      </c>
-      <c r="G7" s="44">
+        <v>79476.74175999999</v>
+      </c>
+      <c r="G7" s="30">
         <f t="shared" si="1"/>
-        <v>121361.79730000001</v>
-      </c>
-      <c r="H7" s="44">
+        <v>123339.43604</v>
+      </c>
+      <c r="H7" s="30">
         <f t="shared" si="1"/>
-        <v>14583.6834</v>
-      </c>
-      <c r="I7" s="44">
+        <v>14723.708999999999</v>
+      </c>
+      <c r="I7" s="30">
         <f t="shared" si="1"/>
-        <v>20679.817080000001</v>
-      </c>
-      <c r="J7" s="44">
+        <v>21088.920320000001</v>
+      </c>
+      <c r="J7" s="30">
         <f t="shared" si="1"/>
-        <v>40892.25591</v>
-      </c>
-      <c r="K7" s="44">
+        <v>41654.570210000005</v>
+      </c>
+      <c r="K7" s="30">
         <f t="shared" si="1"/>
-        <v>147668.81394000002</v>
-      </c>
-      <c r="L7" s="44">
+        <v>148547.27601999999</v>
+      </c>
+      <c r="L7" s="30">
         <f t="shared" si="1"/>
-        <v>42108.110460000004</v>
-      </c>
-      <c r="M7" s="44">
+        <v>42155.296560000003</v>
+      </c>
+      <c r="M7" s="30">
         <f t="shared" si="1"/>
-        <v>23376.64112</v>
-      </c>
-      <c r="N7" s="44">
+        <v>23402.067640000001</v>
+      </c>
+      <c r="N7" s="30">
         <f t="shared" si="1"/>
-        <v>63799.354709999992</v>
-      </c>
-      <c r="O7" s="44">
+        <v>63850.4568</v>
+      </c>
+      <c r="O7" s="30">
         <f t="shared" si="1"/>
-        <v>54851.709759999998</v>
-      </c>
-      <c r="P7" s="44">
+        <v>54908.23425999999</v>
+      </c>
+      <c r="P7" s="30">
         <f t="shared" si="1"/>
-        <v>221048.91769999999</v>
-      </c>
-      <c r="Q7" s="44">
+        <v>221572.79793999999</v>
+      </c>
+      <c r="Q7" s="30">
         <f t="shared" si="1"/>
-        <v>72973.343720000004</v>
-      </c>
-      <c r="R7" s="44">
+        <v>73157.115760000001</v>
+      </c>
+      <c r="R7" s="30">
         <f t="shared" si="1"/>
-        <v>103602.88512000001</v>
-      </c>
-      <c r="S7" s="44">
+        <v>103683.28320000001</v>
+      </c>
+      <c r="S7" s="30">
         <f t="shared" si="1"/>
-        <v>229615.90705999997</v>
-      </c>
-      <c r="T7" s="44">
+        <v>229896.78177999996</v>
+      </c>
+      <c r="T7" s="30">
         <f t="shared" si="1"/>
-        <v>51613.464</v>
-      </c>
-      <c r="U7" s="44">
+        <v>51635.807999999997</v>
+      </c>
+      <c r="U7" s="30">
         <f t="shared" si="1"/>
-        <v>86849.100280000013</v>
-      </c>
-      <c r="V7" s="44">
+        <v>88408.131200000003</v>
+      </c>
+      <c r="V7" s="30">
         <f t="shared" si="1"/>
-        <v>4554.1455999999998</v>
-      </c>
-      <c r="W7" s="44">
+        <v>4647.5734400000001</v>
+      </c>
+      <c r="W7" s="30">
         <f t="shared" si="1"/>
-        <v>1392.1641</v>
-      </c>
-      <c r="X7" s="44">
+        <v>1539.1296</v>
+      </c>
+      <c r="X7" s="30">
         <f t="shared" si="1"/>
-        <v>190814.64998999998</v>
-      </c>
-      <c r="Y7" s="44">
+        <v>195775.26398999998</v>
+      </c>
+      <c r="Y7" s="30">
         <f t="shared" si="1"/>
-        <v>117521.3499</v>
-      </c>
-      <c r="Z7" s="44">
+        <v>130971.6339</v>
+      </c>
+      <c r="Z7" s="30">
         <f t="shared" si="1"/>
-        <v>48782.697140000004</v>
-      </c>
-      <c r="AA7" s="44">
+        <v>97061.248739999995</v>
+      </c>
+      <c r="AA7" s="30">
         <f t="shared" si="1"/>
-        <v>11672.074199999999</v>
-      </c>
-      <c r="AB7" s="44">
+        <v>12443.724479999999</v>
+      </c>
+      <c r="AB7" s="30">
         <f t="shared" si="1"/>
-        <v>3472.61292</v>
-      </c>
-      <c r="AC7" s="44">
+        <v>5887.5299699999996</v>
+      </c>
+      <c r="AC7" s="30">
         <f t="shared" si="1"/>
-        <v>59868.027519999996</v>
-      </c>
-      <c r="AD7" s="44">
+        <v>59973.734239999998</v>
+      </c>
+      <c r="AD7" s="30">
         <f t="shared" si="1"/>
-        <v>55342.472399999999</v>
-      </c>
-      <c r="AE7" s="44">
+        <v>57578.655599999991</v>
+      </c>
+      <c r="AE7" s="30">
         <f t="shared" si="1"/>
-        <v>9843.952299999999</v>
-      </c>
-      <c r="AF7" s="44">
+        <v>16737.868029999998</v>
+      </c>
+      <c r="AF7" s="30">
         <f t="shared" si="1"/>
-        <v>127511.21208</v>
-      </c>
-      <c r="AG7" s="44">
+        <v>130764.69294000001</v>
+      </c>
+      <c r="AG7" s="30">
         <f t="shared" si="1"/>
-        <v>2318.7074400000001</v>
-      </c>
-      <c r="AH7" s="44">
+        <v>2659.5693600000004</v>
+      </c>
+      <c r="AH7" s="30">
         <f t="shared" si="1"/>
-        <v>10863.285839999999</v>
-      </c>
-      <c r="AI7" s="44">
+        <v>17540.495279999999</v>
+      </c>
+      <c r="AI7" s="30">
         <f t="shared" si="1"/>
-        <v>2730.3393299999998</v>
-      </c>
-      <c r="AJ7" s="44">
+        <v>4721.3129399999998</v>
+      </c>
+      <c r="AJ7" s="30">
         <f t="shared" si="1"/>
-        <v>8447.6024600000001</v>
-      </c>
-      <c r="AK7" s="44">
+        <v>15277.967859999999</v>
+      </c>
+      <c r="AK7" s="30">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -9269,296 +9271,296 @@
       <c r="A8" t="s">
         <v>157</v>
       </c>
-      <c r="B8" s="44">
+      <c r="B8" s="30">
         <f>B5-B7</f>
-        <v>409695.18240000005</v>
-      </c>
-      <c r="C8" s="44">
+        <v>407881.61823999998</v>
+      </c>
+      <c r="C8" s="30">
         <f t="shared" ref="C8:AK8" si="2">C5-C7</f>
-        <v>279497.17784000002</v>
-      </c>
-      <c r="D8" s="44">
+        <v>279429.24855999998</v>
+      </c>
+      <c r="D8" s="30">
         <f t="shared" si="2"/>
-        <v>58876.571940000002</v>
-      </c>
-      <c r="E8" s="44">
+        <v>58873.459989999996</v>
+      </c>
+      <c r="E8" s="30">
         <f t="shared" si="2"/>
-        <v>84878.599280000009</v>
-      </c>
-      <c r="F8" s="44">
+        <v>84877.923299999995</v>
+      </c>
+      <c r="F8" s="30">
         <f t="shared" si="2"/>
-        <v>884548.64272</v>
-      </c>
-      <c r="G8" s="44">
+        <v>877640.25824</v>
+      </c>
+      <c r="G8" s="30">
         <f t="shared" si="2"/>
-        <v>102385.70269999999</v>
-      </c>
-      <c r="H8" s="44">
+        <v>101539.06396</v>
+      </c>
+      <c r="H8" s="30">
         <f t="shared" si="2"/>
-        <v>94737.416600000011</v>
-      </c>
-      <c r="I8" s="44">
+        <v>94555.591</v>
+      </c>
+      <c r="I8" s="30">
         <f t="shared" si="2"/>
-        <v>242333.08292000002</v>
-      </c>
-      <c r="J8" s="44">
+        <v>241233.27967999995</v>
+      </c>
+      <c r="J8" s="30">
         <f t="shared" si="2"/>
-        <v>421576.84409000003</v>
-      </c>
-      <c r="K8" s="44">
+        <v>419117.32978999999</v>
+      </c>
+      <c r="K8" s="30">
         <f t="shared" si="2"/>
-        <v>666086.48605999991</v>
-      </c>
-      <c r="L8" s="44">
+        <v>664272.02398000006</v>
+      </c>
+      <c r="L8" s="30">
         <f t="shared" si="2"/>
-        <v>210856.38954</v>
-      </c>
-      <c r="M8" s="44">
+        <v>210803.30343999999</v>
+      </c>
+      <c r="M8" s="30">
         <f t="shared" si="2"/>
-        <v>111772.85888</v>
-      </c>
-      <c r="N8" s="44">
+        <v>111758.13236000002</v>
+      </c>
+      <c r="N8" s="30">
         <f t="shared" si="2"/>
-        <v>195316.14528999999</v>
-      </c>
-      <c r="O8" s="44">
+        <v>195324.3432</v>
+      </c>
+      <c r="O8" s="30">
         <f t="shared" si="2"/>
-        <v>334257.99024000001</v>
-      </c>
-      <c r="P8" s="44">
+        <v>334185.36573999998</v>
+      </c>
+      <c r="P8" s="30">
         <f t="shared" si="2"/>
-        <v>325140.1823000001</v>
-      </c>
-      <c r="Q8" s="44">
+        <v>323996.00205999997</v>
+      </c>
+      <c r="Q8" s="30">
         <f t="shared" si="2"/>
-        <v>114644.75628</v>
-      </c>
-      <c r="R8" s="44">
+        <v>114351.38424000003</v>
+      </c>
+      <c r="R8" s="30">
         <f t="shared" si="2"/>
-        <v>309746.41487999994</v>
-      </c>
-      <c r="S8" s="44">
+        <v>309707.81679999997</v>
+      </c>
+      <c r="S8" s="30">
         <f t="shared" si="2"/>
-        <v>638315.49294000003</v>
-      </c>
-      <c r="T8" s="44">
+        <v>637753.21822000004</v>
+      </c>
+      <c r="T8" s="30">
         <f t="shared" si="2"/>
-        <v>215120.53599999999</v>
-      </c>
-      <c r="U8" s="44">
+        <v>215087.19200000001</v>
+      </c>
+      <c r="U8" s="30">
         <f t="shared" si="2"/>
-        <v>237952.29971999995</v>
-      </c>
-      <c r="V8" s="44">
+        <v>235732.96879999997</v>
+      </c>
+      <c r="V8" s="30">
         <f t="shared" si="2"/>
-        <v>475679.75439999998</v>
-      </c>
-      <c r="W8" s="44">
+        <v>475668.42655999999</v>
+      </c>
+      <c r="W8" s="30">
         <f t="shared" si="2"/>
-        <v>1351866.5359000002</v>
-      </c>
-      <c r="X8" s="44">
+        <v>1351884.5704000001</v>
+      </c>
+      <c r="X8" s="30">
         <f t="shared" si="2"/>
-        <v>2730230.3500100002</v>
-      </c>
-      <c r="Y8" s="44">
+        <v>2719957.5360099999</v>
+      </c>
+      <c r="Y8" s="30">
         <f t="shared" si="2"/>
-        <v>1017653.7500999998</v>
-      </c>
-      <c r="Z8" s="44">
+        <v>992781.56609999994</v>
+      </c>
+      <c r="Z8" s="30">
         <f t="shared" si="2"/>
-        <v>920408.70286000008</v>
-      </c>
-      <c r="AA8" s="44">
+        <v>865899.45126000012</v>
+      </c>
+      <c r="AA8" s="30">
         <f t="shared" si="2"/>
-        <v>606128.92579999997</v>
-      </c>
-      <c r="AB8" s="44">
+        <v>605250.57552000007</v>
+      </c>
+      <c r="AB8" s="30">
         <f t="shared" si="2"/>
-        <v>616618.88708000013</v>
-      </c>
-      <c r="AC8" s="44">
+        <v>612122.57003000006</v>
+      </c>
+      <c r="AC8" s="30">
         <f t="shared" si="2"/>
-        <v>551520.77248000004</v>
-      </c>
-      <c r="AD8" s="44">
+        <v>551268.66576</v>
+      </c>
+      <c r="AD8" s="30">
         <f t="shared" si="2"/>
-        <v>2158891.7276000003</v>
-      </c>
-      <c r="AE8" s="44">
+        <v>2154803.2443999997</v>
+      </c>
+      <c r="AE8" s="30">
         <f t="shared" si="2"/>
-        <v>2998478.8476999998</v>
-      </c>
-      <c r="AF8" s="44">
+        <v>2988697.9319699998</v>
+      </c>
+      <c r="AF8" s="30">
         <f t="shared" si="2"/>
-        <v>3100093.0879199998</v>
-      </c>
-      <c r="AG8" s="44">
+        <v>3094383.9070599996</v>
+      </c>
+      <c r="AG8" s="30">
         <f t="shared" si="2"/>
-        <v>2508889.3925599996</v>
-      </c>
-      <c r="AH8" s="44">
+        <v>2508902.9306399999</v>
+      </c>
+      <c r="AH8" s="30">
         <f t="shared" si="2"/>
-        <v>1302764.6141599999</v>
-      </c>
-      <c r="AI8" s="44">
+        <v>1277859.1047200002</v>
+      </c>
+      <c r="AI8" s="30">
         <f t="shared" si="2"/>
-        <v>2187571.4606700004</v>
-      </c>
-      <c r="AJ8" s="44">
+        <v>2184593.1870599999</v>
+      </c>
+      <c r="AJ8" s="30">
         <f t="shared" si="2"/>
-        <v>798325.59753999999</v>
-      </c>
-      <c r="AK8" s="44">
+        <v>786320.53214000002</v>
+      </c>
+      <c r="AK8" s="30">
         <f t="shared" si="2"/>
         <v>21351.7</v>
       </c>
     </row>
     <row r="9" spans="1:37" x14ac:dyDescent="0.25">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="B9" s="45">
+      <c r="B9" s="31">
         <f>B8/B5</f>
-        <v>0.92262302400514529</v>
-      </c>
-      <c r="C9" s="45">
+        <v>0.92010228335058653</v>
+      </c>
+      <c r="C9" s="31">
         <f t="shared" ref="C9:AK9" si="3">C8/C5</f>
-        <v>0.64141076415168385</v>
-      </c>
-      <c r="D9" s="45">
+        <v>0.64126458772425854</v>
+      </c>
+      <c r="D9" s="31">
         <f t="shared" si="3"/>
-        <v>0.88596150688435782</v>
-      </c>
-      <c r="E9" s="45">
+        <v>0.88574540701724291</v>
+      </c>
+      <c r="E9" s="31">
         <f t="shared" si="3"/>
-        <v>0.98287694589803065</v>
-      </c>
-      <c r="F9" s="45">
+        <v>0.98282700871921347</v>
+      </c>
+      <c r="F9" s="31">
         <f t="shared" si="3"/>
-        <v>0.92129629594680051</v>
-      </c>
-      <c r="G9" s="45">
+        <v>0.91696235490540867</v>
+      </c>
+      <c r="G9" s="31">
         <f t="shared" si="3"/>
-        <v>0.45759484552900032</v>
-      </c>
-      <c r="H9" s="45">
+        <v>0.45152855413034149</v>
+      </c>
+      <c r="H9" s="31">
         <f t="shared" si="3"/>
-        <v>0.86659772541622804</v>
-      </c>
-      <c r="I9" s="45">
+        <v>0.86526534302470826</v>
+      </c>
+      <c r="I9" s="31">
         <f t="shared" si="3"/>
-        <v>0.92137337339727443</v>
-      </c>
-      <c r="J9" s="45">
+        <v>0.91960680293166186</v>
+      </c>
+      <c r="J9" s="31">
         <f t="shared" si="3"/>
-        <v>0.91157840402742585</v>
-      </c>
-      <c r="K9" s="45">
+        <v>0.90959828450910307</v>
+      </c>
+      <c r="K9" s="31">
         <f t="shared" si="3"/>
-        <v>0.81853412943669912</v>
-      </c>
-      <c r="L9" s="45">
+        <v>0.81724440349780081</v>
+      </c>
+      <c r="L9" s="31">
         <f t="shared" si="3"/>
-        <v>0.83354142395474462</v>
-      </c>
-      <c r="M9" s="45">
+        <v>0.83335100463079737</v>
+      </c>
+      <c r="M9" s="31">
         <f t="shared" si="3"/>
-        <v>0.82703124229094449</v>
-      </c>
-      <c r="N9" s="45">
+        <v>0.82685681406212785</v>
+      </c>
+      <c r="N9" s="31">
         <f t="shared" si="3"/>
-        <v>0.75378024583631631</v>
-      </c>
-      <c r="O9" s="45">
+        <v>0.75363940938702367</v>
+      </c>
+      <c r="O9" s="31">
         <f t="shared" si="3"/>
-        <v>0.85903278751467771</v>
-      </c>
-      <c r="P9" s="45">
+        <v>0.8588816822995804</v>
+      </c>
+      <c r="P9" s="31">
         <f t="shared" si="3"/>
-        <v>0.59528866888775345</v>
-      </c>
-      <c r="Q9" s="45">
+        <v>0.59386827483536453</v>
+      </c>
+      <c r="Q9" s="31">
         <f t="shared" si="3"/>
-        <v>0.61105381772867329</v>
-      </c>
-      <c r="R9" s="45">
+        <v>0.6098464029097348</v>
+      </c>
+      <c r="R9" s="31">
         <f t="shared" si="3"/>
-        <v>0.74935754065629234</v>
-      </c>
-      <c r="S9" s="45">
+        <v>0.74918840004054266</v>
+      </c>
+      <c r="S9" s="31">
         <f t="shared" si="3"/>
-        <v>0.73544463645398706</v>
-      </c>
-      <c r="T9" s="45">
+        <v>0.73503511579553971</v>
+      </c>
+      <c r="T9" s="31">
         <f t="shared" si="3"/>
-        <v>0.80649836916178663</v>
-      </c>
-      <c r="U9" s="45">
+        <v>0.80640661660224278</v>
+      </c>
+      <c r="U9" s="31">
         <f t="shared" si="3"/>
-        <v>0.7326086024259747</v>
-      </c>
-      <c r="V9" s="45">
+        <v>0.72725417665331549</v>
+      </c>
+      <c r="V9" s="31">
         <f t="shared" si="3"/>
-        <v>0.99051681774235434</v>
-      </c>
-      <c r="W9" s="45">
+        <v>0.99032392541576797</v>
+      </c>
+      <c r="W9" s="31">
         <f t="shared" si="3"/>
-        <v>0.99897125058202108</v>
-      </c>
-      <c r="X9" s="45">
+        <v>0.99886278805373363</v>
+      </c>
+      <c r="X9" s="31">
         <f t="shared" si="3"/>
-        <v>0.93467589510260884</v>
-      </c>
-      <c r="Y9" s="45">
+        <v>0.93285555384567476</v>
+      </c>
+      <c r="Y9" s="31">
         <f t="shared" si="3"/>
-        <v>0.89647293188513377</v>
-      </c>
-      <c r="Z9" s="45">
+        <v>0.88345160316339921</v>
+      </c>
+      <c r="Z9" s="31">
         <f t="shared" si="3"/>
-        <v>0.94966660131321845</v>
-      </c>
-      <c r="AA9" s="45">
+        <v>0.89920538944112682</v>
+      </c>
+      <c r="AA9" s="31">
         <f t="shared" si="3"/>
-        <v>0.98110706489630151</v>
-      </c>
-      <c r="AB9" s="45">
+        <v>0.97985455834706592</v>
+      </c>
+      <c r="AB9" s="31">
         <f t="shared" si="3"/>
-        <v>0.99439983789489139</v>
-      </c>
-      <c r="AC9" s="45">
+        <v>0.99047340816921914</v>
+      </c>
+      <c r="AC9" s="31">
         <f t="shared" si="3"/>
-        <v>0.90207863225495788</v>
-      </c>
-      <c r="AD9" s="45">
+        <v>0.9018822414151898</v>
+      </c>
+      <c r="AD9" s="31">
         <f t="shared" si="3"/>
-        <v>0.97500604389544709</v>
-      </c>
-      <c r="AE9" s="45">
+        <v>0.97397435967090484</v>
+      </c>
+      <c r="AE9" s="31">
         <f t="shared" si="3"/>
-        <v>0.99672776063127266</v>
-      </c>
-      <c r="AF9" s="45">
+        <v>0.99443080167275577</v>
+      </c>
+      <c r="AF9" s="31">
         <f t="shared" si="3"/>
-        <v>0.9604935425076736</v>
-      </c>
-      <c r="AG9" s="45">
+        <v>0.95945467661862149</v>
+      </c>
+      <c r="AG9" s="31">
         <f t="shared" si="3"/>
-        <v>0.99907665659409106</v>
-      </c>
-      <c r="AH9" s="45">
+        <v>0.99894106980813735</v>
+      </c>
+      <c r="AH9" s="31">
         <f t="shared" si="3"/>
-        <v>0.99173031736003781</v>
-      </c>
-      <c r="AI9" s="45">
+        <v>0.98645939424406193</v>
+      </c>
+      <c r="AI9" s="31">
         <f t="shared" si="3"/>
-        <v>0.998753441498336</v>
-      </c>
-      <c r="AJ9" s="45">
+        <v>0.99784347432038656</v>
+      </c>
+      <c r="AJ9" s="31">
         <f t="shared" si="3"/>
-        <v>0.98952914839015482</v>
-      </c>
-      <c r="AK9" s="45">
+        <v>0.98094062319228392</v>
+      </c>
+      <c r="AK9" s="31">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -9697,148 +9699,148 @@
       </c>
     </row>
     <row r="2" spans="1:37" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="46" t="s">
+      <c r="A2" s="32" t="s">
         <v>158</v>
       </c>
       <c r="B2" s="16">
         <f>Calculations!B9</f>
-        <v>0.92262302400514529</v>
+        <v>0.92010228335058653</v>
       </c>
       <c r="C2" s="16">
         <f>Calculations!C9</f>
-        <v>0.64141076415168385</v>
+        <v>0.64126458772425854</v>
       </c>
       <c r="D2" s="16">
         <f>Calculations!D9</f>
-        <v>0.88596150688435782</v>
+        <v>0.88574540701724291</v>
       </c>
       <c r="E2" s="16">
         <f>Calculations!E9</f>
-        <v>0.98287694589803065</v>
+        <v>0.98282700871921347</v>
       </c>
       <c r="F2" s="16">
         <f>Calculations!F9</f>
-        <v>0.92129629594680051</v>
+        <v>0.91696235490540867</v>
       </c>
       <c r="G2" s="16">
         <f>Calculations!G9</f>
-        <v>0.45759484552900032</v>
+        <v>0.45152855413034149</v>
       </c>
       <c r="H2" s="16">
         <f>Calculations!H9</f>
-        <v>0.86659772541622804</v>
+        <v>0.86526534302470826</v>
       </c>
       <c r="I2" s="16">
         <f>Calculations!I9</f>
-        <v>0.92137337339727443</v>
+        <v>0.91960680293166186</v>
       </c>
       <c r="J2" s="16">
         <f>Calculations!J9</f>
-        <v>0.91157840402742585</v>
+        <v>0.90959828450910307</v>
       </c>
       <c r="K2" s="16">
         <f>Calculations!K9</f>
-        <v>0.81853412943669912</v>
+        <v>0.81724440349780081</v>
       </c>
       <c r="L2" s="16">
         <f>Calculations!L9</f>
-        <v>0.83354142395474462</v>
+        <v>0.83335100463079737</v>
       </c>
       <c r="M2" s="16">
         <f>Calculations!M9</f>
-        <v>0.82703124229094449</v>
+        <v>0.82685681406212785</v>
       </c>
       <c r="N2" s="16">
         <f>Calculations!N9</f>
-        <v>0.75378024583631631</v>
+        <v>0.75363940938702367</v>
       </c>
       <c r="O2" s="16">
         <f>Calculations!O9</f>
-        <v>0.85903278751467771</v>
+        <v>0.8588816822995804</v>
       </c>
       <c r="P2" s="16">
         <f>Calculations!P9</f>
-        <v>0.59528866888775345</v>
+        <v>0.59386827483536453</v>
       </c>
       <c r="Q2" s="16">
         <f>Calculations!Q9</f>
-        <v>0.61105381772867329</v>
+        <v>0.6098464029097348</v>
       </c>
       <c r="R2" s="16">
         <f>Calculations!R9</f>
-        <v>0.74935754065629234</v>
+        <v>0.74918840004054266</v>
       </c>
       <c r="S2" s="16">
         <f>Calculations!S9</f>
-        <v>0.73544463645398706</v>
+        <v>0.73503511579553971</v>
       </c>
       <c r="T2" s="16">
         <f>Calculations!T9</f>
-        <v>0.80649836916178663</v>
+        <v>0.80640661660224278</v>
       </c>
       <c r="U2" s="16">
         <f>Calculations!U9</f>
-        <v>0.7326086024259747</v>
+        <v>0.72725417665331549</v>
       </c>
       <c r="V2" s="16">
         <f>Calculations!V9</f>
-        <v>0.99051681774235434</v>
+        <v>0.99032392541576797</v>
       </c>
       <c r="W2" s="16">
         <f>Calculations!W9</f>
-        <v>0.99897125058202108</v>
+        <v>0.99886278805373363</v>
       </c>
       <c r="X2" s="16">
         <f>Calculations!X9</f>
-        <v>0.93467589510260884</v>
+        <v>0.93285555384567476</v>
       </c>
       <c r="Y2" s="16">
         <f>Calculations!Y9</f>
-        <v>0.89647293188513377</v>
+        <v>0.88345160316339921</v>
       </c>
       <c r="Z2" s="16">
         <f>Calculations!Z9</f>
-        <v>0.94966660131321845</v>
+        <v>0.89920538944112682</v>
       </c>
       <c r="AA2" s="16">
         <f>Calculations!AA9</f>
-        <v>0.98110706489630151</v>
+        <v>0.97985455834706592</v>
       </c>
       <c r="AB2" s="16">
         <f>Calculations!AB9</f>
-        <v>0.99439983789489139</v>
+        <v>0.99047340816921914</v>
       </c>
       <c r="AC2" s="16">
         <f>Calculations!AC9</f>
-        <v>0.90207863225495788</v>
+        <v>0.9018822414151898</v>
       </c>
       <c r="AD2" s="16">
         <f>Calculations!AD9</f>
-        <v>0.97500604389544709</v>
+        <v>0.97397435967090484</v>
       </c>
       <c r="AE2" s="16">
         <f>Calculations!AE9</f>
-        <v>0.99672776063127266</v>
+        <v>0.99443080167275577</v>
       </c>
       <c r="AF2" s="16">
         <f>Calculations!AF9</f>
-        <v>0.9604935425076736</v>
+        <v>0.95945467661862149</v>
       </c>
       <c r="AG2" s="16">
         <f>Calculations!AG9</f>
-        <v>0.99907665659409106</v>
+        <v>0.99894106980813735</v>
       </c>
       <c r="AH2" s="16">
         <f>Calculations!AH9</f>
-        <v>0.99173031736003781</v>
+        <v>0.98645939424406193</v>
       </c>
       <c r="AI2" s="16">
         <f>Calculations!AI9</f>
-        <v>0.998753441498336</v>
+        <v>0.99784347432038656</v>
       </c>
       <c r="AJ2" s="16">
         <f>Calculations!AJ9</f>
-        <v>0.98952914839015482</v>
+        <v>0.98094062319228392</v>
       </c>
       <c r="AK2" s="16">
         <f>Calculations!AK9</f>

</xml_diff>